<commit_message>
Fixed a bug so that only rank 0 opens the output file. Also fixed the 1024 core zerr input
</commit_message>
<xml_diff>
--- a/run/zerr_suite/Zerr_Suite.xlsx
+++ b/run/zerr_suite/Zerr_Suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Cores</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Sweep time</t>
+  </si>
+  <si>
+    <t>Cab</t>
   </si>
 </sst>
 </file>
@@ -263,25 +266,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0456006921130108</c:v>
+                  <c:v>1.0020202803825926</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.50504343667809037</c:v>
+                  <c:v>1.0008588346969218</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.99800926698816583</c:v>
+                  <c:v>0.98559700875625544</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.96791429147497099</c:v>
+                  <c:v>0.9209114405394967</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.93743231968188023</c:v>
+                  <c:v>0.90816353435774233</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.82673565719742925</c:v>
+                  <c:v>0.85053585833365342</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.92840880121662839</c:v>
+                  <c:v>0.19016735374950922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -673,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:S28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,71 +1423,70 @@
         <v>13</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:E20" si="0">C6/C12</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D19:S19" si="0">D6/(2*D21)</f>
         <v>4</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19:S20" si="1">F6/F12</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19:H19" si="2">G6/G12</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="J19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="K19">
-        <f t="shared" si="1"/>
-        <v>32</v>
+        <f t="shared" si="0"/>
+        <v>64</v>
       </c>
       <c r="L19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="M19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="N19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="O19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="P19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>256</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="1"/>
-        <v>256</v>
+        <f t="shared" si="0"/>
+        <v>512</v>
       </c>
       <c r="R19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>512</v>
       </c>
       <c r="S19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>768</v>
       </c>
     </row>
@@ -1493,27 +1495,26 @@
         <v>14</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" ref="D20:S20" si="1">D7/(2*D21)</f>
+        <v>4</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G20">
-        <f t="shared" ref="G20:H20" si="3">G7/G13</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="H20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I20">
@@ -1522,7 +1523,7 @@
       </c>
       <c r="J20">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="K20">
         <f t="shared" si="1"/>
@@ -1530,7 +1531,7 @@
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="M20">
         <f t="shared" si="1"/>
@@ -1546,7 +1547,7 @@
       </c>
       <c r="P20">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="Q20">
         <f t="shared" si="1"/>
@@ -1554,11 +1555,11 @@
       </c>
       <c r="R20">
         <f t="shared" si="1"/>
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="S20">
         <f t="shared" si="1"/>
-        <v>256</v>
+        <v>512</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -1566,71 +1567,70 @@
         <v>22</v>
       </c>
       <c r="C21">
-        <f>MIN(C12:C13)/2</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:S21" si="4">MIN(D12:D13)/2</f>
+        <f t="shared" ref="D21:S21" si="2">MIN(D12:D13)/2</f>
         <v>4</v>
       </c>
       <c r="E21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="F21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="G21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="L21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="M21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="N21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="R21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1651,59 +1651,59 @@
         <v>64</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="F22:S22" si="5">F8</f>
+        <f t="shared" ref="F22:S22" si="3">F8</f>
         <v>64</v>
       </c>
       <c r="G22">
-        <f t="shared" ref="G22:H22" si="6">G8</f>
+        <f t="shared" ref="G22:H22" si="4">G8</f>
         <v>128</v>
       </c>
       <c r="H22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="I22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="J22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>256</v>
       </c>
       <c r="K22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>256</v>
       </c>
       <c r="L22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>256</v>
       </c>
       <c r="M22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>512</v>
       </c>
       <c r="N22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>512</v>
       </c>
       <c r="O22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>512</v>
       </c>
       <c r="P22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1024</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1024</v>
       </c>
       <c r="R22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1024</v>
       </c>
       <c r="S22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1024</v>
       </c>
     </row>
@@ -1768,71 +1768,71 @@
         <v>17</v>
       </c>
       <c r="C25">
-        <f>C6/(2*C21)</f>
+        <f>C9</f>
         <v>2</v>
       </c>
       <c r="D25">
-        <f>D6/(2*D21)</f>
+        <f t="shared" ref="D25:S25" si="5">D9</f>
         <v>4</v>
       </c>
       <c r="E25">
-        <f>E6/(2*E21)</f>
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>4</v>
       </c>
       <c r="F25">
-        <f>F6/(2*F21)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="G25">
-        <f>G6/(2*G21)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="H25">
-        <f>H6/(2*H21)</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="I25">
-        <f>I6/(2*I21)</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J25">
-        <f>J6/(2*J21)</f>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="K25">
-        <f>K6/(2*K21)</f>
-        <v>64</v>
+        <f t="shared" si="5"/>
+        <v>32</v>
       </c>
       <c r="L25">
-        <f>L6/(2*L21)</f>
+        <f t="shared" si="5"/>
         <v>64</v>
       </c>
       <c r="M25">
-        <f>M6/(2*M21)</f>
+        <f t="shared" si="5"/>
         <v>64</v>
       </c>
       <c r="N25">
-        <f>N6/(2*N21)</f>
+        <f t="shared" si="5"/>
         <v>128</v>
       </c>
       <c r="O25">
-        <f>O6/(2*O21)</f>
+        <f t="shared" si="5"/>
         <v>128</v>
       </c>
       <c r="P25">
-        <f>P6/(2*P21)</f>
+        <f t="shared" si="5"/>
         <v>256</v>
       </c>
       <c r="Q25">
-        <f>Q6/(2*Q21)</f>
-        <v>512</v>
+        <f t="shared" si="5"/>
+        <v>256</v>
       </c>
       <c r="R25">
-        <f>R6/(2*R21)</f>
+        <f t="shared" si="5"/>
         <v>512</v>
       </c>
       <c r="S25">
-        <f>S6/(2*S21)</f>
+        <f t="shared" si="5"/>
         <v>768</v>
       </c>
     </row>
@@ -1897,72 +1897,72 @@
         <v>19</v>
       </c>
       <c r="C28">
-        <f>C7/(2*C21)</f>
+        <f>C10</f>
         <v>2</v>
       </c>
       <c r="D28">
-        <f>D7/(2*D21)</f>
-        <v>4</v>
+        <f t="shared" ref="D28:S28" si="6">D10</f>
+        <v>2</v>
       </c>
       <c r="E28">
-        <f>E7/(2*E21)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="F28">
-        <f>F7/(2*F21)</f>
-        <v>8</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="G28">
-        <f t="shared" ref="G28:S28" si="7">G7/(2*G21)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="H28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="I28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="J28">
-        <f t="shared" si="7"/>
-        <v>32</v>
+        <f t="shared" si="6"/>
+        <v>16</v>
       </c>
       <c r="K28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="L28">
-        <f t="shared" si="7"/>
-        <v>64</v>
+        <f t="shared" si="6"/>
+        <v>32</v>
       </c>
       <c r="M28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="N28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="O28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>128</v>
       </c>
       <c r="P28">
-        <f t="shared" si="7"/>
-        <v>256</v>
+        <f t="shared" si="6"/>
+        <v>128</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>256</v>
       </c>
       <c r="R28">
-        <f t="shared" si="7"/>
-        <v>512</v>
+        <f t="shared" si="6"/>
+        <v>256</v>
       </c>
       <c r="S28">
-        <f t="shared" si="7"/>
-        <v>512</v>
+        <f t="shared" si="6"/>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -1982,59 +1982,59 @@
         <v>32</v>
       </c>
       <c r="F30">
-        <f t="shared" ref="F30:S30" si="8">F31/2</f>
+        <f t="shared" ref="F30:S30" si="7">F31/2</f>
         <v>32</v>
       </c>
       <c r="G30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
       <c r="H30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
       <c r="I30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
       <c r="J30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>128</v>
       </c>
       <c r="K30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>128</v>
       </c>
       <c r="L30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>128</v>
       </c>
       <c r="M30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>256</v>
       </c>
       <c r="N30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>256</v>
       </c>
       <c r="O30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>256</v>
       </c>
       <c r="P30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>512</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>512</v>
       </c>
       <c r="R30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>512</v>
       </c>
       <c r="S30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>512</v>
       </c>
     </row>
@@ -2055,59 +2055,59 @@
         <v>64</v>
       </c>
       <c r="F31">
-        <f t="shared" ref="F31:S31" si="9">F8</f>
+        <f t="shared" ref="F31:S31" si="8">F8</f>
         <v>64</v>
       </c>
       <c r="G31">
-        <f t="shared" ref="G31:H31" si="10">G8</f>
+        <f t="shared" ref="G31:H31" si="9">G8</f>
         <v>128</v>
       </c>
       <c r="H31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>128</v>
       </c>
       <c r="I31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>128</v>
       </c>
       <c r="J31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>256</v>
       </c>
       <c r="K31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>256</v>
       </c>
       <c r="L31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>256</v>
       </c>
       <c r="M31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>512</v>
       </c>
       <c r="N31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>512</v>
       </c>
       <c r="O31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>512</v>
       </c>
       <c r="P31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1024</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1024</v>
       </c>
       <c r="R31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1024</v>
       </c>
       <c r="S31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1024</v>
       </c>
     </row>
@@ -2120,63 +2120,63 @@
         <v>1</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:S35" si="11">E5/16</f>
+        <f t="shared" ref="E35:S35" si="10">E5/16</f>
         <v>2</v>
       </c>
       <c r="F35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="G35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="H35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="I35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>32</v>
       </c>
       <c r="J35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="K35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>128</v>
       </c>
       <c r="L35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>256</v>
       </c>
       <c r="M35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>512</v>
       </c>
       <c r="N35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1024</v>
       </c>
       <c r="O35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>2048</v>
       </c>
       <c r="P35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>4096</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>8192</v>
       </c>
       <c r="R35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16384</v>
       </c>
       <c r="S35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>24576</v>
       </c>
     </row>
@@ -2236,12 +2236,17 @@
         <v>0.34127099999999999</v>
       </c>
     </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="42" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="1">
         <v>8</v>
       </c>
       <c r="D42">
-        <v>0.31683899999999998</v>
+        <v>0.30998799999999999</v>
       </c>
       <c r="E42">
         <f>$D$42/D42</f>
@@ -2253,11 +2258,11 @@
         <v>16</v>
       </c>
       <c r="D43">
-        <v>0.154888</v>
+        <v>0.309363</v>
       </c>
       <c r="E43">
-        <f t="shared" ref="E43:E49" si="12">$D$42/D43</f>
-        <v>2.0456006921130108</v>
+        <f t="shared" ref="E43:E49" si="11">$D$42/D43</f>
+        <v>1.0020202803825926</v>
       </c>
     </row>
     <row r="44" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2265,11 +2270,11 @@
         <v>32</v>
       </c>
       <c r="D44">
-        <v>0.62734999999999996</v>
+        <v>0.309722</v>
       </c>
       <c r="E44">
-        <f t="shared" si="12"/>
-        <v>0.50504343667809037</v>
+        <f t="shared" si="11"/>
+        <v>1.0008588346969218</v>
       </c>
     </row>
     <row r="45" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2277,11 +2282,11 @@
         <v>64</v>
       </c>
       <c r="D45">
-        <v>0.317471</v>
+        <v>0.31451800000000002</v>
       </c>
       <c r="E45">
-        <f t="shared" si="12"/>
-        <v>0.99800926698816583</v>
+        <f t="shared" si="11"/>
+        <v>0.98559700875625544</v>
       </c>
     </row>
     <row r="46" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2289,11 +2294,11 @@
         <v>128</v>
       </c>
       <c r="D46">
-        <v>0.32734200000000002</v>
+        <v>0.33661000000000002</v>
       </c>
       <c r="E46">
-        <f t="shared" si="12"/>
-        <v>0.96791429147497099</v>
+        <f t="shared" si="11"/>
+        <v>0.9209114405394967</v>
       </c>
     </row>
     <row r="47" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2301,11 +2306,11 @@
         <v>256</v>
       </c>
       <c r="D47">
-        <v>0.33798600000000001</v>
+        <v>0.341335</v>
       </c>
       <c r="E47">
-        <f t="shared" si="12"/>
-        <v>0.93743231968188023</v>
+        <f t="shared" si="11"/>
+        <v>0.90816353435774233</v>
       </c>
     </row>
     <row r="48" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2313,11 +2318,11 @@
         <v>512</v>
       </c>
       <c r="D48">
-        <v>0.383241</v>
+        <v>0.36446200000000001</v>
       </c>
       <c r="E48">
-        <f t="shared" si="12"/>
-        <v>0.82673565719742925</v>
+        <f t="shared" si="11"/>
+        <v>0.85053585833365342</v>
       </c>
     </row>
     <row r="49" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2325,11 +2330,11 @@
         <v>1024</v>
       </c>
       <c r="D49">
-        <v>0.34127099999999999</v>
+        <v>1.63008</v>
       </c>
       <c r="E49">
-        <f t="shared" si="12"/>
-        <v>0.92840880121662839</v>
+        <f t="shared" si="11"/>
+        <v>0.19016735374950922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding the excel sheet to the repo
</commit_message>
<xml_diff>
--- a/run/zerr_suite/Zerr_Suite.xlsx
+++ b/run/zerr_suite/Zerr_Suite.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Zerr" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Cores</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Cab</t>
+  </si>
+  <si>
+    <t>unknowns per core</t>
+  </si>
+  <si>
+    <t>cells/core</t>
   </si>
 </sst>
 </file>
@@ -284,7 +290,7 @@
                   <c:v>0.85053585833365342</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.19016735374950922</c:v>
+                  <c:v>0.70900424504135251</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -299,11 +305,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210998336"/>
-        <c:axId val="210998912"/>
+        <c:axId val="228502336"/>
+        <c:axId val="228502912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210998336"/>
+        <c:axId val="228502336"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -314,12 +320,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210998912"/>
+        <c:crossAx val="228502912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210998912"/>
+        <c:axId val="228502912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -330,7 +336,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210998336"/>
+        <c:crossAx val="228502336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -676,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,6 +2117,152 @@
         <v>1024</v>
       </c>
     </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B33" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33">
+        <f>C15*C16*8*C12*C24*C13*C27*C14*C30</f>
+        <v>327680</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ref="D33:S33" si="10">D15*D16*8*D12*D24*D13*D27*D14*D30</f>
+        <v>327680</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="10"/>
+        <v>327680</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34">
+        <f>C12*C13*C14*C24*C27*C30</f>
+        <v>4096</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ref="D34:S34" si="11">D12*D13*D14*D24*D27*D30</f>
+        <v>4096</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="11"/>
+        <v>4096</v>
+      </c>
+    </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>24</v>
@@ -2120,63 +2272,63 @@
         <v>1</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:S35" si="10">E5/16</f>
+        <f t="shared" ref="E35:S35" si="12">E5/16</f>
         <v>2</v>
       </c>
       <c r="F35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="G35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="H35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>16</v>
       </c>
       <c r="I35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>32</v>
       </c>
       <c r="J35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>64</v>
       </c>
       <c r="K35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>128</v>
       </c>
       <c r="L35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>256</v>
       </c>
       <c r="M35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>512</v>
       </c>
       <c r="N35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1024</v>
       </c>
       <c r="O35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2048</v>
       </c>
       <c r="P35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4096</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>8192</v>
       </c>
       <c r="R35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>16384</v>
       </c>
       <c r="S35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>24576</v>
       </c>
     </row>
@@ -2261,7 +2413,7 @@
         <v>0.309363</v>
       </c>
       <c r="E43">
-        <f t="shared" ref="E43:E49" si="11">$D$42/D43</f>
+        <f t="shared" ref="E43:E49" si="13">$D$42/D43</f>
         <v>1.0020202803825926</v>
       </c>
     </row>
@@ -2273,7 +2425,7 @@
         <v>0.309722</v>
       </c>
       <c r="E44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.0008588346969218</v>
       </c>
     </row>
@@ -2285,7 +2437,7 @@
         <v>0.31451800000000002</v>
       </c>
       <c r="E45">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.98559700875625544</v>
       </c>
     </row>
@@ -2297,7 +2449,7 @@
         <v>0.33661000000000002</v>
       </c>
       <c r="E46">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.9209114405394967</v>
       </c>
     </row>
@@ -2309,7 +2461,7 @@
         <v>0.341335</v>
       </c>
       <c r="E47">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.90816353435774233</v>
       </c>
     </row>
@@ -2321,7 +2473,7 @@
         <v>0.36446200000000001</v>
       </c>
       <c r="E48">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.85053585833365342</v>
       </c>
     </row>
@@ -2330,11 +2482,11 @@
         <v>1024</v>
       </c>
       <c r="D49">
-        <v>1.63008</v>
+        <v>0.43721599999999999</v>
       </c>
       <c r="E49">
-        <f t="shared" si="11"/>
-        <v>0.19016735374950922</v>
+        <f t="shared" si="13"/>
+        <v>0.70900424504135251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing order(# of task) scaling problems.
</commit_message>
<xml_diff>
--- a/run/zerr_suite/Zerr_Suite.xlsx
+++ b/run/zerr_suite/Zerr_Suite.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="-255" windowWidth="20805" windowHeight="5490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="299"/>
   </bookViews>
   <sheets>
     <sheet name="Zerr" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -56,10 +56,16 @@
     <t>cellsets per processor</t>
   </si>
   <si>
+    <t>SimpleLD parameters</t>
+  </si>
+  <si>
     <t>num_pin_x</t>
   </si>
   <si>
     <t>num_pin_y</t>
+  </si>
+  <si>
+    <t>refinement</t>
   </si>
   <si>
     <t>z_planes</t>
@@ -83,25 +89,19 @@
     <t>num_cellsets_z</t>
   </si>
   <si>
-    <t>refinement</t>
+    <t>unknowns per core</t>
   </si>
   <si>
-    <t>SimpleLD parameters</t>
+    <t>cells/core</t>
   </si>
   <si>
     <t># of Nodes</t>
   </si>
   <si>
-    <t>Sweep time</t>
-  </si>
-  <si>
     <t>Cab</t>
   </si>
   <si>
-    <t>unknowns per core</t>
-  </si>
-  <si>
-    <t>cells/core</t>
+    <t>Vulcan</t>
   </si>
 </sst>
 </file>
@@ -111,26 +111,29 @@
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -143,7 +146,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -157,6 +160,15 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
@@ -164,40 +176,102 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF878787"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF4A7EBB"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -210,17 +284,10 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -229,6 +296,29 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cab</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cab</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="4A7EBB"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="7"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Zerr!$C$42:$C$49</c:f>
@@ -266,7 +356,7 @@
             <c:numRef>
               <c:f>Zerr!$E$42:$E$49</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -295,7 +385,125 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>vulcan</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vulcan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="FF420E"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Zerr!$C$42:$C$53</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>16384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Zerr!$H$42:$H$53</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98433598919967336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96998277509738029</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95201101582812564</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.90264900662251657</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.88993801201383671</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.87727801728101218</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.71347534398769341</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.698974358974359</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.68045432223542179</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.37641662777774021</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.36330572470209116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -305,13 +513,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228502336"/>
-        <c:axId val="228502912"/>
+        <c:axId val="179016768"/>
+        <c:axId val="179017344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="228502336"/>
+        <c:axId val="179016768"/>
         <c:scaling>
-          <c:logBase val="2"/>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -320,36 +528,81 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="228502912"/>
-        <c:crosses val="autoZero"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="878787"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="179017344"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="228502912"/>
+        <c:axId val="179017344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="878787"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="228502336"/>
-        <c:crosses val="autoZero"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="878787"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="179016768"/>
+        <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -360,22 +613,22 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:colOff>131760</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>67320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
+      <xdr:colOff>436320</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="2" name="Chart 7"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -680,18 +933,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:S49"/>
+  <dimension ref="A5:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="20.85546875"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -748,685 +1003,685 @@
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
         <v>32</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>32</v>
       </c>
-      <c r="E6" s="4">
-        <v>64</v>
-      </c>
-      <c r="F6" s="2">
-        <v>64</v>
-      </c>
-      <c r="G6" s="4">
-        <v>64</v>
-      </c>
-      <c r="H6" s="4">
-        <v>128</v>
-      </c>
-      <c r="I6" s="2">
-        <v>128</v>
-      </c>
-      <c r="J6" s="2">
-        <v>128</v>
-      </c>
-      <c r="K6" s="2">
-        <v>256</v>
-      </c>
-      <c r="L6" s="2">
-        <v>256</v>
-      </c>
-      <c r="M6" s="2">
-        <v>256</v>
-      </c>
-      <c r="N6" s="2">
-        <v>512</v>
-      </c>
-      <c r="O6" s="2">
-        <v>512</v>
-      </c>
-      <c r="P6" s="2">
-        <v>512</v>
-      </c>
-      <c r="Q6" s="2">
+      <c r="E6" s="3">
+        <v>64</v>
+      </c>
+      <c r="F6" s="3">
+        <v>64</v>
+      </c>
+      <c r="G6" s="3">
+        <v>64</v>
+      </c>
+      <c r="H6" s="3">
+        <v>128</v>
+      </c>
+      <c r="I6" s="3">
+        <v>128</v>
+      </c>
+      <c r="J6" s="3">
+        <v>128</v>
+      </c>
+      <c r="K6" s="3">
+        <v>256</v>
+      </c>
+      <c r="L6" s="3">
+        <v>256</v>
+      </c>
+      <c r="M6" s="3">
+        <v>256</v>
+      </c>
+      <c r="N6" s="3">
+        <v>512</v>
+      </c>
+      <c r="O6" s="3">
+        <v>512</v>
+      </c>
+      <c r="P6" s="3">
+        <v>512</v>
+      </c>
+      <c r="Q6" s="3">
         <v>1024</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="3">
         <v>1024</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="3">
         <v>1536</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
         <v>32</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>32</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>32</v>
       </c>
-      <c r="F7" s="2">
-        <v>64</v>
-      </c>
-      <c r="G7" s="4">
-        <v>64</v>
-      </c>
-      <c r="H7" s="4">
-        <v>64</v>
-      </c>
-      <c r="I7" s="2">
-        <v>128</v>
-      </c>
-      <c r="J7" s="2">
-        <v>128</v>
-      </c>
-      <c r="K7" s="2">
-        <v>128</v>
-      </c>
-      <c r="L7" s="2">
-        <v>256</v>
-      </c>
-      <c r="M7" s="2">
-        <v>256</v>
-      </c>
-      <c r="N7" s="2">
-        <v>256</v>
-      </c>
-      <c r="O7" s="2">
-        <v>512</v>
-      </c>
-      <c r="P7" s="2">
-        <v>512</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>512</v>
-      </c>
-      <c r="R7" s="2">
+      <c r="F7" s="3">
+        <v>64</v>
+      </c>
+      <c r="G7" s="3">
+        <v>64</v>
+      </c>
+      <c r="H7" s="3">
+        <v>64</v>
+      </c>
+      <c r="I7" s="3">
+        <v>128</v>
+      </c>
+      <c r="J7" s="3">
+        <v>128</v>
+      </c>
+      <c r="K7" s="3">
+        <v>128</v>
+      </c>
+      <c r="L7" s="3">
+        <v>256</v>
+      </c>
+      <c r="M7" s="3">
+        <v>256</v>
+      </c>
+      <c r="N7" s="3">
+        <v>256</v>
+      </c>
+      <c r="O7" s="3">
+        <v>512</v>
+      </c>
+      <c r="P7" s="3">
+        <v>512</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>512</v>
+      </c>
+      <c r="R7" s="3">
         <v>1024</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="3">
         <v>1024</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>32</v>
       </c>
-      <c r="D8" s="4">
-        <v>64</v>
-      </c>
-      <c r="E8" s="4">
-        <v>64</v>
-      </c>
-      <c r="F8" s="2">
-        <v>64</v>
-      </c>
-      <c r="G8" s="4">
-        <v>128</v>
-      </c>
-      <c r="H8" s="4">
-        <v>128</v>
-      </c>
-      <c r="I8" s="2">
-        <v>128</v>
-      </c>
-      <c r="J8" s="2">
-        <v>256</v>
-      </c>
-      <c r="K8" s="2">
-        <v>256</v>
-      </c>
-      <c r="L8" s="2">
-        <v>256</v>
-      </c>
-      <c r="M8" s="2">
-        <v>512</v>
-      </c>
-      <c r="N8" s="2">
-        <v>512</v>
-      </c>
-      <c r="O8" s="2">
-        <v>512</v>
-      </c>
-      <c r="P8" s="2">
+      <c r="D8" s="3">
+        <v>64</v>
+      </c>
+      <c r="E8" s="3">
+        <v>64</v>
+      </c>
+      <c r="F8" s="3">
+        <v>64</v>
+      </c>
+      <c r="G8" s="3">
+        <v>128</v>
+      </c>
+      <c r="H8" s="3">
+        <v>128</v>
+      </c>
+      <c r="I8" s="3">
+        <v>128</v>
+      </c>
+      <c r="J8" s="3">
+        <v>256</v>
+      </c>
+      <c r="K8" s="3">
+        <v>256</v>
+      </c>
+      <c r="L8" s="3">
+        <v>256</v>
+      </c>
+      <c r="M8" s="3">
+        <v>512</v>
+      </c>
+      <c r="N8" s="3">
+        <v>512</v>
+      </c>
+      <c r="O8" s="3">
+        <v>512</v>
+      </c>
+      <c r="P8" s="3">
         <v>1024</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8" s="3">
         <v>1024</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" s="3">
         <v>1024</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8" s="3">
         <v>1024</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4">
-        <v>4</v>
-      </c>
-      <c r="E9" s="4">
-        <v>4</v>
-      </c>
-      <c r="F9" s="4">
-        <v>8</v>
-      </c>
-      <c r="G9" s="4">
-        <v>8</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3">
+        <v>8</v>
+      </c>
+      <c r="H9" s="3">
         <v>16</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>16</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <v>32</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="3">
         <v>32</v>
       </c>
-      <c r="L9" s="4">
-        <v>64</v>
-      </c>
-      <c r="M9" s="4">
-        <v>64</v>
-      </c>
-      <c r="N9" s="4">
-        <v>128</v>
-      </c>
-      <c r="O9" s="4">
-        <v>128</v>
-      </c>
-      <c r="P9" s="4">
-        <v>256</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>256</v>
-      </c>
-      <c r="R9" s="4">
-        <v>512</v>
-      </c>
-      <c r="S9" s="4">
+      <c r="L9" s="3">
+        <v>64</v>
+      </c>
+      <c r="M9" s="3">
+        <v>64</v>
+      </c>
+      <c r="N9" s="3">
+        <v>128</v>
+      </c>
+      <c r="O9" s="3">
+        <v>128</v>
+      </c>
+      <c r="P9" s="3">
+        <v>256</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>256</v>
+      </c>
+      <c r="R9" s="3">
+        <v>512</v>
+      </c>
+      <c r="S9" s="3">
         <v>768</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="4">
-        <v>2</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4">
-        <v>4</v>
-      </c>
-      <c r="F10" s="4">
-        <v>4</v>
-      </c>
-      <c r="G10" s="4">
-        <v>8</v>
-      </c>
-      <c r="H10" s="4">
-        <v>8</v>
-      </c>
-      <c r="I10" s="4">
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>8</v>
+      </c>
+      <c r="H10" s="3">
+        <v>8</v>
+      </c>
+      <c r="I10" s="3">
         <v>16</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>16</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <v>32</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="3">
         <v>32</v>
       </c>
-      <c r="M10" s="4">
-        <v>64</v>
-      </c>
-      <c r="N10" s="4">
-        <v>64</v>
-      </c>
-      <c r="O10" s="4">
-        <v>128</v>
-      </c>
-      <c r="P10" s="4">
-        <v>128</v>
-      </c>
-      <c r="Q10" s="4">
-        <v>256</v>
-      </c>
-      <c r="R10" s="4">
-        <v>256</v>
-      </c>
-      <c r="S10" s="4">
+      <c r="M10" s="3">
+        <v>64</v>
+      </c>
+      <c r="N10" s="3">
+        <v>64</v>
+      </c>
+      <c r="O10" s="3">
+        <v>128</v>
+      </c>
+      <c r="P10" s="3">
+        <v>128</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>256</v>
+      </c>
+      <c r="R10" s="3">
+        <v>256</v>
+      </c>
+      <c r="S10" s="3">
         <v>256</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="7">
-        <v>2</v>
-      </c>
-      <c r="D11" s="7">
-        <v>2</v>
-      </c>
-      <c r="E11" s="7">
-        <v>2</v>
-      </c>
-      <c r="F11" s="7">
-        <v>2</v>
-      </c>
-      <c r="G11" s="7">
-        <v>2</v>
-      </c>
-      <c r="H11" s="7">
-        <v>2</v>
-      </c>
-      <c r="I11" s="7">
-        <v>2</v>
-      </c>
-      <c r="J11" s="7">
-        <v>2</v>
-      </c>
-      <c r="K11" s="7">
-        <v>2</v>
-      </c>
-      <c r="L11" s="7">
-        <v>2</v>
-      </c>
-      <c r="M11" s="7">
-        <v>2</v>
-      </c>
-      <c r="N11" s="7">
-        <v>2</v>
-      </c>
-      <c r="O11" s="7">
-        <v>2</v>
-      </c>
-      <c r="P11" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="7">
-        <v>2</v>
-      </c>
-      <c r="R11" s="7">
-        <v>2</v>
-      </c>
-      <c r="S11" s="7">
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2</v>
+      </c>
+      <c r="I11" s="4">
+        <v>2</v>
+      </c>
+      <c r="J11" s="4">
+        <v>2</v>
+      </c>
+      <c r="K11" s="4">
+        <v>2</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2</v>
+      </c>
+      <c r="M11" s="4">
+        <v>2</v>
+      </c>
+      <c r="N11" s="4">
+        <v>2</v>
+      </c>
+      <c r="O11" s="4">
+        <v>2</v>
+      </c>
+      <c r="P11" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>2</v>
+      </c>
+      <c r="R11" s="4">
+        <v>2</v>
+      </c>
+      <c r="S11" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="4">
         <v>16</v>
       </c>
-      <c r="D12" s="7">
-        <v>8</v>
-      </c>
-      <c r="E12" s="7">
+      <c r="D12" s="4">
+        <v>8</v>
+      </c>
+      <c r="E12" s="4">
         <v>16</v>
       </c>
-      <c r="F12" s="7">
-        <v>8</v>
-      </c>
-      <c r="G12" s="7">
-        <v>8</v>
-      </c>
-      <c r="H12" s="7">
-        <v>8</v>
-      </c>
-      <c r="I12" s="7">
-        <v>8</v>
-      </c>
-      <c r="J12" s="7">
-        <v>4</v>
-      </c>
-      <c r="K12" s="7">
-        <v>8</v>
-      </c>
-      <c r="L12" s="7">
-        <v>4</v>
-      </c>
-      <c r="M12" s="7">
-        <v>4</v>
-      </c>
-      <c r="N12" s="7">
-        <v>4</v>
-      </c>
-      <c r="O12" s="7">
-        <v>4</v>
-      </c>
-      <c r="P12" s="7">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="7">
-        <v>4</v>
-      </c>
-      <c r="R12" s="7">
-        <v>2</v>
-      </c>
-      <c r="S12" s="7">
+      <c r="F12" s="4">
+        <v>8</v>
+      </c>
+      <c r="G12" s="4">
+        <v>8</v>
+      </c>
+      <c r="H12" s="4">
+        <v>8</v>
+      </c>
+      <c r="I12" s="4">
+        <v>8</v>
+      </c>
+      <c r="J12" s="4">
+        <v>4</v>
+      </c>
+      <c r="K12" s="4">
+        <v>8</v>
+      </c>
+      <c r="L12" s="4">
+        <v>4</v>
+      </c>
+      <c r="M12" s="4">
+        <v>4</v>
+      </c>
+      <c r="N12" s="4">
+        <v>4</v>
+      </c>
+      <c r="O12" s="4">
+        <v>4</v>
+      </c>
+      <c r="P12" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>4</v>
+      </c>
+      <c r="R12" s="4">
+        <v>2</v>
+      </c>
+      <c r="S12" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="7">
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4">
         <v>16</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="4">
         <v>16</v>
       </c>
-      <c r="E13" s="7">
-        <v>8</v>
-      </c>
-      <c r="F13" s="7">
+      <c r="E13" s="4">
+        <v>8</v>
+      </c>
+      <c r="F13" s="4">
         <v>16</v>
       </c>
-      <c r="G13" s="7">
-        <v>8</v>
-      </c>
-      <c r="H13" s="7">
-        <v>8</v>
-      </c>
-      <c r="I13" s="7">
-        <v>8</v>
-      </c>
-      <c r="J13" s="7">
-        <v>8</v>
-      </c>
-      <c r="K13" s="7">
-        <v>4</v>
-      </c>
-      <c r="L13" s="7">
-        <v>8</v>
-      </c>
-      <c r="M13" s="7">
-        <v>4</v>
-      </c>
-      <c r="N13" s="7">
-        <v>4</v>
-      </c>
-      <c r="O13" s="7">
-        <v>4</v>
-      </c>
-      <c r="P13" s="7">
-        <v>4</v>
-      </c>
-      <c r="Q13" s="7">
-        <v>2</v>
-      </c>
-      <c r="R13" s="7">
-        <v>4</v>
-      </c>
-      <c r="S13" s="7">
+      <c r="G13" s="4">
+        <v>8</v>
+      </c>
+      <c r="H13" s="4">
+        <v>8</v>
+      </c>
+      <c r="I13" s="4">
+        <v>8</v>
+      </c>
+      <c r="J13" s="4">
+        <v>8</v>
+      </c>
+      <c r="K13" s="4">
+        <v>4</v>
+      </c>
+      <c r="L13" s="4">
+        <v>8</v>
+      </c>
+      <c r="M13" s="4">
+        <v>4</v>
+      </c>
+      <c r="N13" s="4">
+        <v>4</v>
+      </c>
+      <c r="O13" s="4">
+        <v>4</v>
+      </c>
+      <c r="P13" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>2</v>
+      </c>
+      <c r="R13" s="4">
+        <v>4</v>
+      </c>
+      <c r="S13" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="10">
-        <v>1</v>
-      </c>
-      <c r="D14" s="10">
-        <v>1</v>
-      </c>
-      <c r="E14" s="10">
-        <v>1</v>
-      </c>
-      <c r="F14" s="10">
-        <v>1</v>
-      </c>
-      <c r="G14" s="10">
-        <v>1</v>
-      </c>
-      <c r="H14" s="10">
-        <v>1</v>
-      </c>
-      <c r="I14" s="10">
-        <v>1</v>
-      </c>
-      <c r="J14" s="10">
-        <v>1</v>
-      </c>
-      <c r="K14" s="10">
-        <v>1</v>
-      </c>
-      <c r="L14" s="10">
-        <v>1</v>
-      </c>
-      <c r="M14" s="10">
-        <v>1</v>
-      </c>
-      <c r="N14" s="10">
-        <v>1</v>
-      </c>
-      <c r="O14" s="10">
-        <v>1</v>
-      </c>
-      <c r="P14" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="10">
-        <v>1</v>
-      </c>
-      <c r="R14" s="10">
-        <v>1</v>
-      </c>
-      <c r="S14" s="10">
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
+        <v>1</v>
+      </c>
+      <c r="I14" s="5">
+        <v>1</v>
+      </c>
+      <c r="J14" s="5">
+        <v>1</v>
+      </c>
+      <c r="K14" s="5">
+        <v>1</v>
+      </c>
+      <c r="L14" s="5">
+        <v>1</v>
+      </c>
+      <c r="M14" s="5">
+        <v>1</v>
+      </c>
+      <c r="N14" s="5">
+        <v>1</v>
+      </c>
+      <c r="O14" s="5">
+        <v>1</v>
+      </c>
+      <c r="P14" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>1</v>
+      </c>
+      <c r="R14" s="5">
+        <v>1</v>
+      </c>
+      <c r="S14" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="7">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7">
-        <v>1</v>
-      </c>
-      <c r="E15" s="7">
-        <v>1</v>
-      </c>
-      <c r="F15" s="7">
-        <v>1</v>
-      </c>
-      <c r="G15" s="7">
-        <v>1</v>
-      </c>
-      <c r="H15" s="7">
-        <v>1</v>
-      </c>
-      <c r="I15" s="7">
-        <v>1</v>
-      </c>
-      <c r="J15" s="7">
-        <v>1</v>
-      </c>
-      <c r="K15" s="7">
-        <v>1</v>
-      </c>
-      <c r="L15" s="7">
-        <v>1</v>
-      </c>
-      <c r="M15" s="7">
-        <v>1</v>
-      </c>
-      <c r="N15" s="7">
-        <v>1</v>
-      </c>
-      <c r="O15" s="7">
-        <v>1</v>
-      </c>
-      <c r="P15" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="5">
-        <v>1</v>
-      </c>
-      <c r="R15" s="5">
-        <v>1</v>
-      </c>
-      <c r="S15" s="5">
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4">
+        <v>1</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1</v>
+      </c>
+      <c r="N15" s="4">
+        <v>1</v>
+      </c>
+      <c r="O15" s="4">
+        <v>1</v>
+      </c>
+      <c r="P15" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>1</v>
+      </c>
+      <c r="R15" s="7">
+        <v>1</v>
+      </c>
+      <c r="S15" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="5">
         <v>10</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="5">
         <v>10</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="5">
         <v>10</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="5">
         <v>10</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="5">
         <v>10</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="5">
         <v>10</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="5">
         <v>10</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="5">
         <v>10</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="5">
         <v>10</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="5">
         <v>10</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="5">
         <v>10</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="5">
         <v>10</v>
       </c>
-      <c r="O16" s="10">
+      <c r="O16" s="5">
         <v>10</v>
       </c>
-      <c r="P16" s="11">
+      <c r="P16" s="8">
         <v>10</v>
       </c>
-      <c r="Q16" s="11">
+      <c r="Q16" s="8">
         <v>10</v>
       </c>
-      <c r="R16" s="11">
+      <c r="R16" s="8">
         <v>10</v>
       </c>
-      <c r="S16" s="11">
+      <c r="S16" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="4">
         <v>16</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="4">
         <v>32</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="4">
         <v>32</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="4">
         <v>32</v>
       </c>
-      <c r="G17" s="7">
-        <v>64</v>
-      </c>
-      <c r="H17" s="7">
-        <v>64</v>
-      </c>
-      <c r="I17" s="7">
-        <v>64</v>
-      </c>
-      <c r="J17" s="7">
-        <v>128</v>
-      </c>
-      <c r="K17" s="7">
-        <v>128</v>
-      </c>
-      <c r="L17" s="7">
-        <v>128</v>
-      </c>
-      <c r="M17" s="7">
-        <v>256</v>
-      </c>
-      <c r="N17" s="7">
-        <v>256</v>
-      </c>
-      <c r="O17" s="7">
-        <v>256</v>
-      </c>
-      <c r="P17" s="7">
-        <v>512</v>
-      </c>
-      <c r="Q17" s="7">
-        <v>512</v>
-      </c>
-      <c r="R17" s="7">
-        <v>512</v>
-      </c>
-      <c r="S17" s="7">
+      <c r="G17" s="4">
+        <v>64</v>
+      </c>
+      <c r="H17" s="4">
+        <v>64</v>
+      </c>
+      <c r="I17" s="4">
+        <v>64</v>
+      </c>
+      <c r="J17" s="4">
+        <v>128</v>
+      </c>
+      <c r="K17" s="4">
+        <v>128</v>
+      </c>
+      <c r="L17" s="4">
+        <v>128</v>
+      </c>
+      <c r="M17" s="4">
+        <v>256</v>
+      </c>
+      <c r="N17" s="4">
+        <v>256</v>
+      </c>
+      <c r="O17" s="4">
+        <v>256</v>
+      </c>
+      <c r="P17" s="4">
+        <v>512</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>512</v>
+      </c>
+      <c r="R17" s="4">
+        <v>512</v>
+      </c>
+      <c r="S17" s="4">
         <v>512</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -1498,7 +1753,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -1570,7 +1825,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -1642,30 +1897,30 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C22">
-        <f>C8</f>
+        <f t="shared" ref="C22:S22" si="3">C8</f>
         <v>32</v>
       </c>
       <c r="D22">
-        <f>D8</f>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="E22">
-        <f>E8</f>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="F22:S22" si="3">F8</f>
+        <f t="shared" si="3"/>
         <v>64</v>
       </c>
       <c r="G22">
-        <f t="shared" ref="G22:H22" si="4">G8</f>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="H22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="I22">
@@ -1715,7 +1970,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1771,726 +2026,793 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C25">
-        <f>C9</f>
+        <f t="shared" ref="C25:S25" si="4">C9</f>
         <v>2</v>
       </c>
       <c r="D25">
-        <f t="shared" ref="D25:S25" si="5">D9</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E25">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="4"/>
+        <v>256</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="4"/>
+        <v>256</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="4"/>
+        <v>512</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="4"/>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:S28" si="5">C10</f>
+        <v>2</v>
+      </c>
+      <c r="D28">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="E28">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="F28">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="I25">
+      <c r="J28">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="J25">
+      <c r="K28">
         <f t="shared" si="5"/>
         <v>32</v>
       </c>
-      <c r="K25">
+      <c r="L28">
         <f t="shared" si="5"/>
         <v>32</v>
       </c>
-      <c r="L25">
+      <c r="M28">
         <f t="shared" si="5"/>
         <v>64</v>
       </c>
-      <c r="M25">
+      <c r="N28">
         <f t="shared" si="5"/>
         <v>64</v>
       </c>
-      <c r="N25">
+      <c r="O28">
         <f t="shared" si="5"/>
         <v>128</v>
       </c>
-      <c r="O25">
+      <c r="P28">
         <f t="shared" si="5"/>
         <v>128</v>
       </c>
-      <c r="P25">
+      <c r="Q28">
         <f t="shared" si="5"/>
         <v>256</v>
       </c>
-      <c r="Q25">
+      <c r="R28">
         <f t="shared" si="5"/>
         <v>256</v>
       </c>
-      <c r="R25">
+      <c r="S28">
         <f t="shared" si="5"/>
-        <v>512</v>
-      </c>
-      <c r="S25">
-        <f t="shared" si="5"/>
-        <v>768</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
-      <c r="M27">
-        <v>1</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-      <c r="O27">
-        <v>1</v>
-      </c>
-      <c r="P27">
-        <v>1</v>
-      </c>
-      <c r="Q27">
-        <v>1</v>
-      </c>
-      <c r="R27">
-        <v>1</v>
-      </c>
-      <c r="S27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28">
-        <f>C10</f>
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <f t="shared" ref="D28:S28" si="6">D10</f>
-        <v>2</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="6"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:S30" si="6">C31/2</f>
         <v>16</v>
       </c>
-      <c r="J28">
-        <f t="shared" si="6"/>
-        <v>16</v>
-      </c>
-      <c r="K28">
+      <c r="D30">
         <f t="shared" si="6"/>
         <v>32</v>
       </c>
-      <c r="L28">
+      <c r="E30">
         <f t="shared" si="6"/>
         <v>32</v>
       </c>
-      <c r="M28">
+      <c r="F30">
         <f t="shared" si="6"/>
-        <v>64</v>
-      </c>
-      <c r="N28">
+        <v>32</v>
+      </c>
+      <c r="G30">
         <f t="shared" si="6"/>
         <v>64</v>
       </c>
-      <c r="O28">
+      <c r="H30">
         <f t="shared" si="6"/>
-        <v>128</v>
-      </c>
-      <c r="P28">
+        <v>64</v>
+      </c>
+      <c r="I30">
         <f t="shared" si="6"/>
-        <v>128</v>
-      </c>
-      <c r="Q28">
+        <v>64</v>
+      </c>
+      <c r="J30">
         <f t="shared" si="6"/>
-        <v>256</v>
-      </c>
-      <c r="R28">
+        <v>128</v>
+      </c>
+      <c r="K30">
         <f t="shared" si="6"/>
-        <v>256</v>
-      </c>
-      <c r="S28">
+        <v>128</v>
+      </c>
+      <c r="L30">
         <f t="shared" si="6"/>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30">
-        <f>C31/2</f>
-        <v>16</v>
-      </c>
-      <c r="D30">
-        <f>D31/2</f>
-        <v>32</v>
-      </c>
-      <c r="E30">
-        <f>E31/2</f>
-        <v>32</v>
-      </c>
-      <c r="F30">
-        <f t="shared" ref="F30:S30" si="7">F31/2</f>
-        <v>32</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="7"/>
-        <v>64</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="7"/>
-        <v>64</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="7"/>
-        <v>64</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="7"/>
-        <v>128</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="7"/>
-        <v>128</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="7"/>
         <v>128</v>
       </c>
       <c r="M30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>256</v>
       </c>
       <c r="N30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>256</v>
       </c>
       <c r="O30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>256</v>
       </c>
       <c r="P30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>512</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>512</v>
       </c>
       <c r="R30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>512</v>
       </c>
       <c r="S30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>512</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B31" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C31">
-        <f>C8</f>
+        <f t="shared" ref="C31:S31" si="7">C8</f>
         <v>32</v>
       </c>
       <c r="D31">
-        <f>D8</f>
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
       <c r="E31">
-        <f>E8</f>
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
       <c r="F31">
-        <f t="shared" ref="F31:S31" si="8">F8</f>
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
       <c r="G31">
-        <f t="shared" ref="G31:H31" si="9">G8</f>
+        <f t="shared" si="7"/>
         <v>128</v>
       </c>
       <c r="H31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>128</v>
       </c>
       <c r="I31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>128</v>
       </c>
       <c r="J31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>256</v>
       </c>
       <c r="K31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>256</v>
       </c>
       <c r="L31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>256</v>
       </c>
       <c r="M31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>512</v>
       </c>
       <c r="N31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>512</v>
       </c>
       <c r="O31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>512</v>
       </c>
       <c r="P31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1024</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1024</v>
       </c>
       <c r="R31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1024</v>
       </c>
       <c r="S31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1024</v>
       </c>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C33">
-        <f>C15*C16*8*C12*C24*C13*C27*C14*C30</f>
+        <f t="shared" ref="C33:S33" si="8">C15*C16*8*C12*C24*C13*C27*C14*C30</f>
         <v>327680</v>
       </c>
       <c r="D33">
-        <f t="shared" ref="D33:S33" si="10">D15*D16*8*D12*D24*D13*D27*D14*D30</f>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="E33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="F33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="G33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="H33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="I33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="J33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="K33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="L33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="M33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="N33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="O33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="P33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="R33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
       <c r="S33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>327680</v>
       </c>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C34">
-        <f>C12*C13*C14*C24*C27*C30</f>
+        <f t="shared" ref="C34:S34" si="9">C12*C13*C14*C24*C27*C30</f>
         <v>4096</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:S34" si="11">D12*D13*D14*D24*D27*D30</f>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="E34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="F34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="G34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="H34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="I34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="J34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="K34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="L34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="M34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="N34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="O34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="P34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="R34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
       <c r="S34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>4096</v>
       </c>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D35">
-        <f>D5/16</f>
+        <f t="shared" ref="D35:S35" si="10">D5/16</f>
         <v>1</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:S35" si="12">E5/16</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="F35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="G35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="H35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="I35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>32</v>
       </c>
       <c r="J35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="K35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>128</v>
       </c>
       <c r="L35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>256</v>
       </c>
       <c r="M35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>512</v>
       </c>
       <c r="N35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>1024</v>
       </c>
       <c r="O35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>2048</v>
       </c>
       <c r="P35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>4096</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>8192</v>
       </c>
       <c r="R35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>16384</v>
       </c>
       <c r="S35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>24576</v>
       </c>
     </row>
-    <row r="38" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="1">
-        <v>8</v>
-      </c>
-      <c r="D38" s="1">
-        <v>16</v>
-      </c>
-      <c r="E38" s="1">
-        <v>32</v>
-      </c>
-      <c r="F38" s="1">
-        <v>64</v>
-      </c>
-      <c r="G38" s="1">
-        <v>128</v>
-      </c>
-      <c r="H38" s="1">
-        <v>256</v>
-      </c>
-      <c r="I38" s="1">
-        <v>512</v>
-      </c>
-      <c r="J38" s="1">
-        <v>1024</v>
-      </c>
-      <c r="K38" s="1"/>
-    </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39">
-        <v>0.31683899999999998</v>
-      </c>
-      <c r="D39">
-        <v>0.154888</v>
-      </c>
-      <c r="E39">
-        <v>0.62734999999999996</v>
-      </c>
-      <c r="F39">
-        <v>0.317471</v>
-      </c>
-      <c r="G39">
-        <v>0.32734200000000002</v>
-      </c>
-      <c r="H39">
-        <v>0.33798600000000001</v>
-      </c>
-      <c r="I39">
-        <v>0.383241</v>
-      </c>
-      <c r="J39">
-        <v>0.34127099999999999</v>
-      </c>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="1">
+        <v>27</v>
+      </c>
+      <c r="G41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C42" s="10">
         <v>8</v>
       </c>
       <c r="D42">
         <v>0.30998799999999999</v>
       </c>
-      <c r="E42">
-        <f>$D$42/D42</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="1">
+      <c r="E42" s="11">
+        <f t="shared" ref="E42:E49" si="11">$D$42/D42</f>
+        <v>1</v>
+      </c>
+      <c r="G42" s="12">
+        <v>3.33935</v>
+      </c>
+      <c r="H42" s="11">
+        <f t="shared" ref="H42:H53" si="12">$G$42/G42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C43" s="10">
         <v>16</v>
       </c>
       <c r="D43">
         <v>0.309363</v>
       </c>
-      <c r="E43">
-        <f t="shared" ref="E43:E49" si="13">$D$42/D43</f>
+      <c r="E43" s="11">
+        <f t="shared" si="11"/>
         <v>1.0020202803825926</v>
       </c>
-    </row>
-    <row r="44" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="1">
+      <c r="G43" s="12">
+        <v>3.39249</v>
+      </c>
+      <c r="H43" s="11">
+        <f t="shared" si="12"/>
+        <v>0.98433598919967336</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C44" s="10">
         <v>32</v>
       </c>
       <c r="D44">
         <v>0.309722</v>
       </c>
-      <c r="E44">
-        <f t="shared" si="13"/>
+      <c r="E44" s="11">
+        <f t="shared" si="11"/>
         <v>1.0008588346969218</v>
       </c>
-    </row>
-    <row r="45" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="1">
+      <c r="G44" s="12">
+        <v>3.4426899999999998</v>
+      </c>
+      <c r="H44" s="11">
+        <f t="shared" si="12"/>
+        <v>0.96998277509738029</v>
+      </c>
+    </row>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C45" s="10">
         <v>64</v>
       </c>
       <c r="D45">
         <v>0.31451800000000002</v>
       </c>
-      <c r="E45">
-        <f t="shared" si="13"/>
+      <c r="E45" s="11">
+        <f t="shared" si="11"/>
         <v>0.98559700875625544</v>
       </c>
-    </row>
-    <row r="46" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="1">
+      <c r="G45" s="12">
+        <v>3.5076800000000001</v>
+      </c>
+      <c r="H45" s="11">
+        <f t="shared" si="12"/>
+        <v>0.95201101582812564</v>
+      </c>
+    </row>
+    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C46" s="10">
         <v>128</v>
       </c>
       <c r="D46">
         <v>0.33661000000000002</v>
       </c>
-      <c r="E46">
-        <f t="shared" si="13"/>
+      <c r="E46" s="11">
+        <f t="shared" si="11"/>
         <v>0.9209114405394967</v>
       </c>
-    </row>
-    <row r="47" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="1">
+      <c r="G46" s="12">
+        <v>3.6995</v>
+      </c>
+      <c r="H46" s="11">
+        <f t="shared" si="12"/>
+        <v>0.90264900662251657</v>
+      </c>
+    </row>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C47" s="10">
         <v>256</v>
       </c>
       <c r="D47">
         <v>0.341335</v>
       </c>
-      <c r="E47">
-        <f t="shared" si="13"/>
+      <c r="E47" s="11">
+        <f t="shared" si="11"/>
         <v>0.90816353435774233</v>
       </c>
-    </row>
-    <row r="48" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="1">
+      <c r="G47" s="12">
+        <v>3.7523399999999998</v>
+      </c>
+      <c r="H47" s="11">
+        <f t="shared" si="12"/>
+        <v>0.88993801201383671</v>
+      </c>
+    </row>
+    <row r="48" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C48" s="10">
         <v>512</v>
       </c>
       <c r="D48">
         <v>0.36446200000000001</v>
       </c>
-      <c r="E48">
-        <f t="shared" si="13"/>
+      <c r="E48" s="11">
+        <f t="shared" si="11"/>
         <v>0.85053585833365342</v>
       </c>
-    </row>
-    <row r="49" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="1">
+      <c r="G48" s="12">
+        <v>3.8064900000000002</v>
+      </c>
+      <c r="H48" s="11">
+        <f t="shared" si="12"/>
+        <v>0.87727801728101218</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="10">
         <v>1024</v>
       </c>
       <c r="D49">
         <v>0.43721599999999999</v>
       </c>
-      <c r="E49">
-        <f t="shared" si="13"/>
+      <c r="E49" s="11">
+        <f t="shared" si="11"/>
         <v>0.70900424504135251</v>
       </c>
+      <c r="G49" s="12">
+        <v>4.6803999999999997</v>
+      </c>
+      <c r="H49" s="11">
+        <f t="shared" si="12"/>
+        <v>0.71347534398769341</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>2048</v>
+      </c>
+      <c r="E50" s="11"/>
+      <c r="G50" s="12">
+        <v>4.7774999999999999</v>
+      </c>
+      <c r="H50" s="11">
+        <f t="shared" si="12"/>
+        <v>0.698974358974359</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>4096</v>
+      </c>
+      <c r="E51" s="11"/>
+      <c r="G51" s="12">
+        <v>4.9075300000000004</v>
+      </c>
+      <c r="H51" s="11">
+        <f t="shared" si="12"/>
+        <v>0.68045432223542179</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>8192</v>
+      </c>
+      <c r="E52" s="11"/>
+      <c r="G52" s="12">
+        <v>8.8714200000000005</v>
+      </c>
+      <c r="H52" s="11">
+        <f t="shared" si="12"/>
+        <v>0.37641662777774021</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>16384</v>
+      </c>
+      <c r="E53" s="11"/>
+      <c r="G53" s="12">
+        <v>9.1915700000000005</v>
+      </c>
+      <c r="H53" s="11">
+        <f t="shared" si="12"/>
+        <v>0.36330572470209116</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -2499,10 +2821,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1025" width="8.5703125"/>
+  </cols>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>